<commit_message>
Short update on creating list object
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\inhibitiontasks\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E474A26C-5D57-4AA0-8E26-B1FC24D5EDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B64F6F1-8C1C-4A05-91BF-23303DF81686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="364">
   <si>
     <t>study</t>
   </si>
@@ -1074,9 +1074,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nova Southeastern </t>
-  </si>
-  <si>
-    <t>Virginia? 17</t>
   </si>
   <si>
     <t>Penn State Abington</t>
@@ -1554,7 +1551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -1845,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2342,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CF0719-54A4-4A0C-BDDA-03EA16BD7F02}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B15:B35"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2707,7 +2704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>248</v>
       </c>
@@ -2727,13 +2724,13 @@
         <v>98</v>
       </c>
       <c r="I17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>250</v>
       </c>
@@ -2753,16 +2750,13 @@
         <v>98</v>
       </c>
       <c r="I18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K18">
         <v>17</v>
       </c>
-      <c r="O18" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>252</v>
       </c>
@@ -2782,13 +2776,13 @@
         <v>98</v>
       </c>
       <c r="I19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>254</v>
       </c>
@@ -2808,13 +2802,13 @@
         <v>98</v>
       </c>
       <c r="I20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>256</v>
       </c>
@@ -2834,13 +2828,13 @@
         <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>258</v>
       </c>
@@ -2860,13 +2854,13 @@
         <v>98</v>
       </c>
       <c r="I22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>260</v>
       </c>
@@ -2892,7 +2886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>262</v>
       </c>
@@ -2909,16 +2903,16 @@
         <v>82</v>
       </c>
       <c r="G24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>264</v>
       </c>
@@ -2938,13 +2932,13 @@
         <v>98</v>
       </c>
       <c r="I25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>266</v>
       </c>
@@ -2964,13 +2958,13 @@
         <v>98</v>
       </c>
       <c r="I26" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>268</v>
       </c>
@@ -2990,13 +2984,13 @@
         <v>98</v>
       </c>
       <c r="I27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>270</v>
       </c>
@@ -3016,13 +3010,13 @@
         <v>98</v>
       </c>
       <c r="I28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>272</v>
       </c>
@@ -3039,13 +3033,13 @@
         <v>621</v>
       </c>
       <c r="G29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>274</v>
       </c>
@@ -3065,13 +3059,13 @@
         <v>98</v>
       </c>
       <c r="I30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>276</v>
       </c>
@@ -3091,13 +3085,13 @@
         <v>98</v>
       </c>
       <c r="I31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>278</v>
       </c>
@@ -3117,7 +3111,7 @@
         <v>98</v>
       </c>
       <c r="I32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K32">
         <v>31</v>
@@ -3140,10 +3134,10 @@
         <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I33" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K33">
         <v>32</v>
@@ -3169,7 +3163,7 @@
         <v>98</v>
       </c>
       <c r="I34" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.35">
@@ -3192,7 +3186,7 @@
         <v>98</v>
       </c>
       <c r="I35" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.35">
@@ -3228,8 +3222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3684,6 +3678,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="7.453125" customWidth="1"/>
     <col min="2" max="2" width="33.26953125" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" customWidth="1"/>
     <col min="4" max="4" width="15.7265625" customWidth="1"/>
@@ -5563,8 +5558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6530,8 +6525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>